<commit_message>
Voltage read code, expenses and voltage divider for linear reg update
</commit_message>
<xml_diff>
--- a/Expenses.xlsx
+++ b/Expenses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf70330ed7863e8e/Repos/Sound Lights/dancelight/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7E13B45D-5967-4D77-A497-A6D6E89DEB8E}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EEA27299-B938-48BE-B29D-65A9400C8008}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Item</t>
   </si>
@@ -60,6 +60,15 @@
   </si>
   <si>
     <t>NPN BJT transistor</t>
+  </si>
+  <si>
+    <t>Lights, Fets, cables and chargers</t>
+  </si>
+  <si>
+    <t>lots!</t>
+  </si>
+  <si>
+    <t>ali express</t>
   </si>
 </sst>
 </file>
@@ -431,17 +440,17 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.81640625" customWidth="1"/>
-    <col min="2" max="2" width="10.453125" customWidth="1"/>
-    <col min="5" max="5" width="19.26953125" customWidth="1"/>
+    <col min="1" max="1" width="37.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +467,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -473,7 +482,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -488,7 +497,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -503,27 +512,35 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="5">
         <f>SUM(C2:C7)</f>
-        <v>11.5</v>
+        <v>31.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed calculations and updated expense
</commit_message>
<xml_diff>
--- a/Expenses.xlsx
+++ b/Expenses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf70330ed7863e8e/Repos/Sound Lights/dancelight/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EEA27299-B938-48BE-B29D-65A9400C8008}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2AE414B7-93B0-4713-A8AF-8AB9F4595520}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Item</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>ali express</t>
+  </si>
+  <si>
+    <t>digikey prototype order</t>
   </si>
 </sst>
 </file>
@@ -440,7 +443,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,10 +531,18 @@
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="4">
+        <v>50</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E6" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -540,7 +551,7 @@
       </c>
       <c r="C10" s="5">
         <f>SUM(C2:C7)</f>
-        <v>31.5</v>
+        <v>81.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature list and hardware to do
</commit_message>
<xml_diff>
--- a/Expenses.xlsx
+++ b/Expenses.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf70330ed7863e8e/Repos/Sound Lights/dancelight/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmima\OneDrive\Repos\Sound Lights\dancelight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{84E2C6E9-86C6-4739-9AB3-85B519B04E32}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB7BCC4-B92C-49CA-AC7B-D2EADBE41047}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Item</t>
   </si>
@@ -78,6 +78,15 @@
   </si>
   <si>
     <t>Production test run LED order</t>
+  </si>
+  <si>
+    <t>boost test boards</t>
+  </si>
+  <si>
+    <t>2 units</t>
+  </si>
+  <si>
+    <t>amazon</t>
   </si>
 </sst>
 </file>
@@ -449,7 +458,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,13 +574,27 @@
         <v>12</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="5">
-        <f>SUM(C2:C7)</f>
-        <v>151.5</v>
+        <f>SUM(C2:C8)</f>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
board sent for production
</commit_message>
<xml_diff>
--- a/Expenses.xlsx
+++ b/Expenses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmima\OneDrive\Repos\Sound Lights\dancelight\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf70330ed7863e8e/Repos/Sound Lights/dancelight/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB7BCC4-B92C-49CA-AC7B-D2EADBE41047}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="6_{8EA5A5CD-CB2B-4CF0-8CB3-ED078D491002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B6D1EAE0-C93B-4521-A0D2-11CD93BAFFE1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Item</t>
   </si>
@@ -87,6 +87,15 @@
   </si>
   <si>
     <t>amazon</t>
+  </si>
+  <si>
+    <t>Prouction Run</t>
+  </si>
+  <si>
+    <t>30 units SMT</t>
+  </si>
+  <si>
+    <t>JLCPCB</t>
   </si>
 </sst>
 </file>
@@ -134,13 +143,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,13 +598,27 @@
         <v>18</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="6">
+        <v>172</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="5">
-        <f>SUM(C2:C8)</f>
-        <v>157</v>
+        <f>SUM(C2:C9)</f>
+        <v>329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>